<commit_message>
20200311 DB ERD 변경
</commit_message>
<xml_diff>
--- a/working_matirials/DB설계/agency-platform.xlsx
+++ b/working_matirials/DB설계/agency-platform.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="149">
   <si>
     <t>AG_LAW_PARTNER</t>
   </si>
@@ -50,45 +50,48 @@
     <t/>
   </si>
   <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>사업자번호</t>
+  </si>
+  <si>
+    <t>COMPNUM</t>
+  </si>
+  <si>
+    <t>varchar(32)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>varchar(128)</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>varchar(256)</t>
+  </si>
+  <si>
+    <t>상호명</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
     <t>varchar(64)</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>PK</t>
-  </si>
-  <si>
-    <t>사업자번호</t>
-  </si>
-  <si>
-    <t>COMPNUM</t>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>varchar(128)</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>varchar(256)</t>
-  </si>
-  <si>
-    <t>상호명</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
     <t>대표휴대폰</t>
   </si>
   <si>
@@ -149,6 +152,24 @@
     <t>LICENSE</t>
   </si>
   <si>
+    <t>BLOB</t>
+  </si>
+  <si>
+    <t>등록일자</t>
+  </si>
+  <si>
+    <t>REG_DATE</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>수정일자</t>
+  </si>
+  <si>
+    <t>MOD_DATE</t>
+  </si>
+  <si>
     <t>AG_USER</t>
   </si>
   <si>
@@ -158,6 +179,21 @@
     <t>휴대폰</t>
   </si>
   <si>
+    <t>프로필사진</t>
+  </si>
+  <si>
+    <t>PICTURE</t>
+  </si>
+  <si>
+    <t>역할</t>
+  </si>
+  <si>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>varchar(16)</t>
+  </si>
+  <si>
     <t>AG_LAW_FEE</t>
   </si>
   <si>
@@ -167,9 +203,6 @@
     <t>CLASSIFY_T</t>
   </si>
   <si>
-    <t>varchar(16)</t>
-  </si>
-  <si>
     <t>중분류</t>
   </si>
   <si>
@@ -185,9 +218,6 @@
     <t>TERM</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>요금</t>
   </si>
   <si>
@@ -204,6 +234,12 @@
   </si>
   <si>
     <t>AG_LAW_PAYMENT</t>
+  </si>
+  <si>
+    <t>결제ID</t>
+  </si>
+  <si>
+    <t>PAY_ID</t>
   </si>
   <si>
     <t>결제구분</t>
@@ -225,12 +261,6 @@
     <t>결제일시</t>
   </si>
   <si>
-    <t>PAY_DATE</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>AG_LAW_OBJ</t>
   </si>
   <si>
@@ -306,12 +336,6 @@
     <t>varchar(1024)</t>
   </si>
   <si>
-    <t>등록일자</t>
-  </si>
-  <si>
-    <t>REG_DATE</t>
-  </si>
-  <si>
     <t>AG_LAW_AUCTION</t>
   </si>
   <si>
@@ -321,6 +345,12 @@
     <t>USER_ID</t>
   </si>
   <si>
+    <t>경매ID</t>
+  </si>
+  <si>
+    <t>AUCTION_ID</t>
+  </si>
+  <si>
     <t>낙찰기한</t>
   </si>
   <si>
@@ -336,9 +366,6 @@
     <t>응찰일자</t>
   </si>
   <si>
-    <t>AUCTION_DATE</t>
-  </si>
-  <si>
     <t>AG_LAW_LOG</t>
   </si>
   <si>
@@ -378,16 +405,58 @@
     <t>회원구분</t>
   </si>
   <si>
-    <t>USER_TYPE</t>
-  </si>
-  <si>
     <t>서비스번호</t>
   </si>
   <si>
     <t>SERVICE_NO</t>
   </si>
   <si>
-    <t>LOG_DATE</t>
+    <t>SPRING_SESSION</t>
+  </si>
+  <si>
+    <t>PRIMARY_ID</t>
+  </si>
+  <si>
+    <t>char(36)</t>
+  </si>
+  <si>
+    <t>SESSION_ID</t>
+  </si>
+  <si>
+    <t>CREATION_TIME</t>
+  </si>
+  <si>
+    <t>LAST_ACCESS</t>
+  </si>
+  <si>
+    <t>MAX_INACTIVE_INTERVAL</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>EXPIRY_TIME</t>
+  </si>
+  <si>
+    <t>PRINCIPAL_NAME</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>SPRING_SESSION_ATTRIBUTES</t>
+  </si>
+  <si>
+    <t>SESSION_PRIMARY_ID</t>
+  </si>
+  <si>
+    <t>ATTRIBUTE_NAME</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>ATTRIBUTE_BYTES</t>
   </si>
 </sst>
 </file>
@@ -756,7 +825,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H109"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -907,7 +976,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -924,10 +993,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -950,10 +1019,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -976,10 +1045,10 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1002,10 +1071,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1028,16 +1097,16 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -1054,10 +1123,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -1080,10 +1149,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -1106,16 +1175,16 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -1132,10 +1201,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -1158,16 +1227,16 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
         <v>19</v>
@@ -1184,16 +1253,16 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
         <v>19</v>
@@ -1209,99 +1278,99 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -1324,16 +1393,16 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -1350,19 +1419,19 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
@@ -1375,56 +1444,98 @@
       <c r="A27" t="s">
         <v>12</v>
       </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
@@ -1435,19 +1546,19 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
@@ -1461,19 +1572,19 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s">
         <v>19</v>
@@ -1489,105 +1600,105 @@
       <c r="A33" t="s">
         <v>12</v>
       </c>
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
         <v>61</v>
-      </c>
-      <c r="C34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="F37" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G37" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
         <v>19</v>
@@ -1601,22 +1712,22 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G39" t="s">
         <v>12</v>
@@ -1627,19 +1738,19 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="F40" t="s">
         <v>19</v>
@@ -1653,19 +1764,19 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F41" t="s">
         <v>19</v>
@@ -1682,16 +1793,16 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F42" t="s">
         <v>19</v>
@@ -1700,95 +1811,95 @@
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
         <v>12</v>
       </c>
-      <c r="B43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" t="s">
-        <v>58</v>
-      </c>
-      <c r="F43" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="F47" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G47" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48">
@@ -1796,19 +1907,19 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G48" t="s">
         <v>12</v>
@@ -1819,13 +1930,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
@@ -1834,7 +1945,7 @@
         <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G49" t="s">
         <v>12</v>
@@ -1845,22 +1956,22 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" t="s">
         <v>76</v>
       </c>
-      <c r="C50" t="s">
-        <v>77</v>
-      </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G50" t="s">
         <v>12</v>
@@ -1874,25 +1985,25 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
         <v>79</v>
-      </c>
-      <c r="C51" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" t="s">
-        <v>19</v>
-      </c>
-      <c r="G51" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="52">
@@ -1900,16 +2011,16 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" t="s">
         <v>81</v>
       </c>
-      <c r="C52" t="s">
-        <v>82</v>
-      </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
@@ -1926,16 +2037,16 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F53" t="s">
         <v>19</v>
@@ -1951,98 +2062,56 @@
       <c r="A54" t="s">
         <v>12</v>
       </c>
-      <c r="B54" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" t="s">
-        <v>86</v>
-      </c>
-      <c r="D54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" t="s">
-        <v>23</v>
-      </c>
-      <c r="F54" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>55</v>
-      </c>
-      <c r="F55" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" t="s">
-        <v>12</v>
-      </c>
-      <c r="H55" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E56" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H56" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G57" t="s">
         <v>12</v>
@@ -2053,22 +2122,22 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
       </c>
       <c r="E58" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="F58" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G58" t="s">
         <v>12</v>
@@ -2082,16 +2151,16 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
       </c>
       <c r="E59" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F59" t="s">
         <v>19</v>
@@ -2107,53 +2176,95 @@
       <c r="A60" t="s">
         <v>12</v>
       </c>
+      <c r="B60" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D62" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F62" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G62" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H62" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="C63" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
       </c>
       <c r="E63" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F63" t="s">
         <v>19</v>
@@ -2167,22 +2278,22 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="F64" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G64" t="s">
         <v>12</v>
@@ -2193,22 +2304,22 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="F65" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G65" t="s">
         <v>12</v>
@@ -2219,22 +2330,22 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="F66" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G66" t="s">
         <v>12</v>
@@ -2248,16 +2359,16 @@
         <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="F67" t="s">
         <v>19</v>
@@ -2274,16 +2385,16 @@
         <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F68" t="s">
         <v>19</v>
@@ -2300,16 +2411,16 @@
         <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="C69" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="F69" t="s">
         <v>19</v>
@@ -2328,7 +2439,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72">
@@ -2359,22 +2470,22 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F73" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G73" t="s">
         <v>12</v>
@@ -2385,22 +2496,22 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G74" t="s">
         <v>12</v>
@@ -2411,22 +2522,22 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="C75" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="D75" t="s">
         <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="F75" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G75" t="s">
         <v>12</v>
@@ -2437,22 +2548,22 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="C76" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="F76" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G76" t="s">
         <v>12</v>
@@ -2463,13 +2574,13 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B77" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="C77" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
@@ -2478,7 +2589,7 @@
         <v>13</v>
       </c>
       <c r="F77" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G77" t="s">
         <v>12</v>
@@ -2492,16 +2603,16 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C78" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F78" t="s">
         <v>19</v>
@@ -2518,16 +2629,16 @@
         <v>12</v>
       </c>
       <c r="B79" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C79" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="F79" t="s">
         <v>19</v>
@@ -2544,16 +2655,16 @@
         <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C80" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="D80" t="s">
         <v>12</v>
       </c>
       <c r="E80" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
@@ -2567,6 +2678,608 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" t="s">
+        <v>51</v>
+      </c>
+      <c r="C81" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" t="s">
+        <v>50</v>
+      </c>
+      <c r="F81" t="s">
+        <v>19</v>
+      </c>
+      <c r="G81" t="s">
+        <v>12</v>
+      </c>
+      <c r="H81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" t="s">
+        <v>5</v>
+      </c>
+      <c r="F84" t="s">
+        <v>6</v>
+      </c>
+      <c r="G84" t="s">
+        <v>7</v>
+      </c>
+      <c r="H84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" t="s">
+        <v>120</v>
+      </c>
+      <c r="D85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" t="s">
+        <v>12</v>
+      </c>
+      <c r="H85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86" t="s">
+        <v>122</v>
+      </c>
+      <c r="D86" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" t="s">
+        <v>123</v>
+      </c>
+      <c r="F86" t="s">
+        <v>19</v>
+      </c>
+      <c r="G86" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87" t="s">
+        <v>125</v>
+      </c>
+      <c r="D87" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>126</v>
+      </c>
+      <c r="F87" t="s">
+        <v>19</v>
+      </c>
+      <c r="G87" t="s">
+        <v>12</v>
+      </c>
+      <c r="H87" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" t="s">
+        <v>127</v>
+      </c>
+      <c r="C88" t="s">
+        <v>128</v>
+      </c>
+      <c r="D88" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" t="s">
+        <v>129</v>
+      </c>
+      <c r="F88" t="s">
+        <v>19</v>
+      </c>
+      <c r="G88" t="s">
+        <v>12</v>
+      </c>
+      <c r="H88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" t="s">
+        <v>54</v>
+      </c>
+      <c r="C89" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" t="s">
+        <v>19</v>
+      </c>
+      <c r="G89" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" t="s">
+        <v>130</v>
+      </c>
+      <c r="C90" t="s">
+        <v>59</v>
+      </c>
+      <c r="D90" t="s">
+        <v>12</v>
+      </c>
+      <c r="E90" t="s">
+        <v>60</v>
+      </c>
+      <c r="F90" t="s">
+        <v>19</v>
+      </c>
+      <c r="G90" t="s">
+        <v>12</v>
+      </c>
+      <c r="H90" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" t="s">
+        <v>131</v>
+      </c>
+      <c r="C91" t="s">
+        <v>132</v>
+      </c>
+      <c r="D91" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" t="s">
+        <v>19</v>
+      </c>
+      <c r="G91" t="s">
+        <v>12</v>
+      </c>
+      <c r="H91" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" t="s">
+        <v>48</v>
+      </c>
+      <c r="C92" t="s">
+        <v>49</v>
+      </c>
+      <c r="D92" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" t="s">
+        <v>50</v>
+      </c>
+      <c r="F92" t="s">
+        <v>19</v>
+      </c>
+      <c r="G92" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>4</v>
+      </c>
+      <c r="E95" t="s">
+        <v>5</v>
+      </c>
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" t="s">
+        <v>134</v>
+      </c>
+      <c r="C96" t="s">
+        <v>134</v>
+      </c>
+      <c r="D96" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" t="s">
+        <v>135</v>
+      </c>
+      <c r="F96" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" t="s">
+        <v>12</v>
+      </c>
+      <c r="H96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" t="s">
+        <v>136</v>
+      </c>
+      <c r="C97" t="s">
+        <v>136</v>
+      </c>
+      <c r="D97" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97" t="s">
+        <v>135</v>
+      </c>
+      <c r="F97" t="s">
+        <v>19</v>
+      </c>
+      <c r="G97" t="s">
+        <v>12</v>
+      </c>
+      <c r="H97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" t="s">
+        <v>137</v>
+      </c>
+      <c r="C98" t="s">
+        <v>137</v>
+      </c>
+      <c r="D98" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" t="s">
+        <v>90</v>
+      </c>
+      <c r="F98" t="s">
+        <v>19</v>
+      </c>
+      <c r="G98" t="s">
+        <v>12</v>
+      </c>
+      <c r="H98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" t="s">
+        <v>138</v>
+      </c>
+      <c r="C99" t="s">
+        <v>138</v>
+      </c>
+      <c r="D99" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" t="s">
+        <v>90</v>
+      </c>
+      <c r="F99" t="s">
+        <v>19</v>
+      </c>
+      <c r="G99" t="s">
+        <v>12</v>
+      </c>
+      <c r="H99" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" t="s">
+        <v>139</v>
+      </c>
+      <c r="C100" t="s">
+        <v>139</v>
+      </c>
+      <c r="D100" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" t="s">
+        <v>140</v>
+      </c>
+      <c r="F100" t="s">
+        <v>19</v>
+      </c>
+      <c r="G100" t="s">
+        <v>12</v>
+      </c>
+      <c r="H100" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" t="s">
+        <v>141</v>
+      </c>
+      <c r="C101" t="s">
+        <v>141</v>
+      </c>
+      <c r="D101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" t="s">
+        <v>90</v>
+      </c>
+      <c r="F101" t="s">
+        <v>19</v>
+      </c>
+      <c r="G101" t="s">
+        <v>12</v>
+      </c>
+      <c r="H101" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" t="s">
+        <v>142</v>
+      </c>
+      <c r="C102" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" t="s">
+        <v>143</v>
+      </c>
+      <c r="F102" t="s">
+        <v>19</v>
+      </c>
+      <c r="G102" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>3</v>
+      </c>
+      <c r="D105" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" t="s">
+        <v>5</v>
+      </c>
+      <c r="F105" t="s">
+        <v>6</v>
+      </c>
+      <c r="G105" t="s">
+        <v>7</v>
+      </c>
+      <c r="H105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106" t="s">
+        <v>145</v>
+      </c>
+      <c r="C106" t="s">
+        <v>145</v>
+      </c>
+      <c r="D106" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" t="s">
+        <v>135</v>
+      </c>
+      <c r="F106" t="s">
+        <v>14</v>
+      </c>
+      <c r="G106" t="s">
+        <v>12</v>
+      </c>
+      <c r="H106" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107" t="s">
+        <v>146</v>
+      </c>
+      <c r="C107" t="s">
+        <v>146</v>
+      </c>
+      <c r="D107" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" t="s">
+        <v>147</v>
+      </c>
+      <c r="F107" t="s">
+        <v>19</v>
+      </c>
+      <c r="G107" t="s">
+        <v>12</v>
+      </c>
+      <c r="H107" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" t="s">
+        <v>148</v>
+      </c>
+      <c r="C108" t="s">
+        <v>148</v>
+      </c>
+      <c r="D108" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" t="s">
+        <v>47</v>
+      </c>
+      <c r="F108" t="s">
+        <v>19</v>
+      </c>
+      <c r="G108" t="s">
+        <v>12</v>
+      </c>
+      <c r="H108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>